<commit_message>
created Master Results and also finished the Difference Table for Macro
</commit_message>
<xml_diff>
--- a/Results/OLS_Results_Breusch_Pagan.xlsx
+++ b/Results/OLS_Results_Breusch_Pagan.xlsx
@@ -34,430 +34,430 @@
     <t>CLc1 &amp; All</t>
   </si>
   <si>
-    <t>CLc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>CLc1 &amp; USUNR_ECI</t>
+    <t>CLc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>CLc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>Cc1 &amp; All</t>
   </si>
   <si>
-    <t>Cc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>Cc1 &amp; USUNR_ECI</t>
+    <t>Cc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>Cc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>GCc1 &amp; All</t>
   </si>
   <si>
-    <t>GCc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>GCc1 &amp; USUNR_ECI</t>
+    <t>GCc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>GCc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>LCc1 &amp; All</t>
   </si>
   <si>
-    <t>LCc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>LCc1 &amp; USUNR_ECI</t>
+    <t>LCc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>LCc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>NGLNMc1 &amp; All</t>
   </si>
   <si>
-    <t>NGLNMc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>NGLNMc1 &amp; USUNR_ECI</t>
+    <t>NGLNMc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>NGLNMc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>NGc1 &amp; All</t>
   </si>
   <si>
-    <t>NGc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>NGc1 &amp; USUNR_ECI</t>
+    <t>NGc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>NGc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>OJc1 &amp; All</t>
   </si>
   <si>
-    <t>OJc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>OJc1 &amp; USUNR_ECI</t>
+    <t>OJc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>OJc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>PAc1 &amp; All</t>
   </si>
   <si>
-    <t>PAc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>PAc1 &amp; USUNR_ECI</t>
+    <t>PAc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>PAc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>PLc1 &amp; All</t>
   </si>
   <si>
-    <t>PLc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>PLc1 &amp; USUNR_ECI</t>
+    <t>PLc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>PLc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>SIc1 &amp; All</t>
   </si>
   <si>
-    <t>SIc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>SIc1 &amp; USUNR_ECI</t>
+    <t>SIc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>SIc1 &amp; USUNR_DIFF</t>
   </si>
   <si>
     <t>Wc1 &amp; All</t>
   </si>
   <si>
-    <t>Wc1 &amp; CHCPIY_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; CHJOB_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; CHPMI_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; CNCPI_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; CNPMIB_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; EUHICY_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; EUUNR_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; RUCPIY_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; RUUNR_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; USCPI_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; USPMI_ECI</t>
-  </si>
-  <si>
-    <t>Wc1 &amp; USUNR_ECI</t>
+    <t>Wc1 &amp; CHCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; CHJOB_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; CHPMI_LOG</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; CNCPI_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; CNPMIB_LOG</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; EUHICY_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; EUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; RUCPIY_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; RUUNR_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; USCPI_DIFF</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; USPMI_LOG</t>
+  </si>
+  <si>
+    <t>Wc1 &amp; USUNR_DIFF</t>
   </si>
 </sst>
 </file>
@@ -843,16 +843,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>37.74479997886932</v>
+        <v>33.0074363888827</v>
       </c>
       <c r="C2">
-        <v>3.058852457430524E-05</v>
+        <v>0.0003279602121495739</v>
       </c>
       <c r="D2">
-        <v>4.091629462029464</v>
+        <v>3.383235251194027</v>
       </c>
       <c r="E2">
-        <v>0.0001690275492031531</v>
+        <v>0.0009654346429215382</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -860,16 +860,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.941542472672562</v>
+        <v>6.499439520168737</v>
       </c>
       <c r="C3">
-        <v>0.166224285895345</v>
+        <v>0.01052944008607959</v>
       </c>
       <c r="D3">
-        <v>1.940581103410831</v>
+        <v>6.757093182074578</v>
       </c>
       <c r="E3">
-        <v>0.1635011526702723</v>
+        <v>0.01079085041048246</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -877,16 +877,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.006236254855958023</v>
+        <v>24.66282725672805</v>
       </c>
       <c r="C4">
-        <v>0.9377131905826891</v>
+        <v>1.997113754689054E-07</v>
       </c>
       <c r="D4">
-        <v>0.00613263598070131</v>
+        <v>30.5254868856942</v>
       </c>
       <c r="E4">
-        <v>0.9370565154906683</v>
+        <v>6.828870889998061E-07</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -894,16 +894,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>6.449197396192421</v>
+        <v>4.516304236706197</v>
       </c>
       <c r="C5">
-        <v>0.01084188539349614</v>
+        <v>0.03374293276416333</v>
       </c>
       <c r="D5">
-        <v>6.701892679754495</v>
+        <v>4.614711162549404</v>
       </c>
       <c r="E5">
-        <v>0.01110024762683158</v>
+        <v>0.03357327993328092</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -911,16 +911,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>3.08804211239611</v>
+        <v>6.290783881139879</v>
       </c>
       <c r="C6">
-        <v>0.08007641277045338</v>
+        <v>0.01188975781733262</v>
       </c>
       <c r="D6">
-        <v>3.116781002102921</v>
+        <v>6.528164763694855</v>
       </c>
       <c r="E6">
-        <v>0.07886965326903579</v>
+        <v>0.01213673630871049</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -928,16 +928,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.4690393180809993</v>
+        <v>0.2885576752879704</v>
       </c>
       <c r="C7">
-        <v>0.4975434234376129</v>
+        <v>0.5948138095547982</v>
       </c>
       <c r="D7">
-        <v>0.463031830563464</v>
+        <v>0.2844323401569398</v>
       </c>
       <c r="E7">
-        <v>0.4934294594131994</v>
+        <v>0.5911462917175254</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -945,16 +945,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>1.028053236227406</v>
+        <v>2.787963978947818</v>
       </c>
       <c r="C8">
-        <v>0.3146671076179537</v>
+        <v>0.09651898577778836</v>
       </c>
       <c r="D8">
-        <v>1.019654508265755</v>
+        <v>2.806706211098967</v>
       </c>
       <c r="E8">
-        <v>0.3106163454473362</v>
+        <v>0.09497482813746566</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -962,16 +962,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>4.793837378574985</v>
+        <v>0.4380544922315721</v>
       </c>
       <c r="C9">
-        <v>0.02861858899041034</v>
+        <v>0.5121275468163431</v>
       </c>
       <c r="D9">
-        <v>4.91009159406417</v>
+        <v>0.4323317913889864</v>
       </c>
       <c r="E9">
-        <v>0.02856172677362635</v>
+        <v>0.508062966848138</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -979,16 +979,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>1.176939198619746</v>
+        <v>0.06266187276425583</v>
       </c>
       <c r="C10">
-        <v>0.2818552047402043</v>
+        <v>0.8043388577557177</v>
       </c>
       <c r="D10">
-        <v>1.168786803676725</v>
+        <v>0.06164970059897176</v>
       </c>
       <c r="E10">
-        <v>0.2779799958665261</v>
+        <v>0.8023371565082218</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -996,16 +996,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.03430996328920521</v>
+        <v>1.527193125106345</v>
       </c>
       <c r="C11">
-        <v>0.8545596518389958</v>
+        <v>0.2199045324514995</v>
       </c>
       <c r="D11">
-        <v>0.03374777961005029</v>
+        <v>1.521098330630825</v>
       </c>
       <c r="E11">
-        <v>0.8530490410525648</v>
+        <v>0.2165341958993575</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1030,16 +1030,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>5.468635912882842</v>
+        <v>0.00139745646549283</v>
       </c>
       <c r="C13">
-        <v>0.01922759196390495</v>
+        <v>0.970491868494074</v>
       </c>
       <c r="D13">
-        <v>5.63425610847815</v>
+        <v>0.00137418152739083</v>
       </c>
       <c r="E13">
-        <v>0.01936073117091394</v>
+        <v>0.9701799708740392</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1047,16 +1047,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.9771654836241561</v>
+        <v>0.05642285770886879</v>
       </c>
       <c r="C14">
-        <v>0.3270014381817014</v>
+        <v>0.8141494856547589</v>
       </c>
       <c r="D14">
-        <v>0.9687681152626736</v>
+        <v>0.05550857635126672</v>
       </c>
       <c r="E14">
-        <v>0.3228996059188481</v>
+        <v>0.8122418001843205</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1064,16 +1064,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>16.1021826524925</v>
+        <v>17.86100418991273</v>
       </c>
       <c r="C15">
-        <v>0.1857461762729664</v>
+        <v>0.1147710456573746</v>
       </c>
       <c r="D15">
-        <v>1.381913489460831</v>
+        <v>1.559253832782052</v>
       </c>
       <c r="E15">
-        <v>0.1866006149574736</v>
+        <v>0.1199765522081005</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1081,16 +1081,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.02063698818179915</v>
+        <v>2.940148983751172</v>
       </c>
       <c r="C16">
-        <v>0.8869549950523752</v>
+        <v>0.08777012797951168</v>
       </c>
       <c r="D16">
-        <v>0.02029652887232331</v>
+        <v>2.963762358064849</v>
       </c>
       <c r="E16">
-        <v>0.8857722774612047</v>
+        <v>0.08640276329634507</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1098,16 +1098,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>1.007484355529393</v>
+        <v>0.6922269065673126</v>
       </c>
       <c r="C17">
-        <v>0.3195783059121194</v>
+        <v>0.4096640087455574</v>
       </c>
       <c r="D17">
-        <v>0.999080936381508</v>
+        <v>0.6846391719253231</v>
       </c>
       <c r="E17">
-        <v>0.3155062647470518</v>
+        <v>0.4054079585643685</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1115,16 +1115,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>1.831893988771376</v>
+        <v>5.721759733845837</v>
       </c>
       <c r="C18">
-        <v>0.1787978366446603</v>
+        <v>0.01657637202081816</v>
       </c>
       <c r="D18">
-        <v>1.829287935396724</v>
+        <v>5.908103301392663</v>
       </c>
       <c r="E18">
-        <v>0.1759040007003256</v>
+        <v>0.01675592877178504</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1132,16 +1132,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.6825474758487271</v>
+        <v>0.01794811156102583</v>
       </c>
       <c r="C19">
-        <v>0.412966868415538</v>
+        <v>0.8945308878536807</v>
       </c>
       <c r="D19">
-        <v>0.6750110771418557</v>
+        <v>0.0176516164781865</v>
       </c>
       <c r="E19">
-        <v>0.4087108878832157</v>
+        <v>0.8934258524426434</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1149,16 +1149,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.04776275448472145</v>
+        <v>0.341809644758726</v>
       </c>
       <c r="C20">
-        <v>0.8287687796217038</v>
+        <v>0.5626308050859838</v>
       </c>
       <c r="D20">
-        <v>0.04698540984826648</v>
+        <v>0.3370729405299133</v>
       </c>
       <c r="E20">
-        <v>0.8270030079681733</v>
+        <v>0.558786518575535</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1166,16 +1166,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.09876356550960974</v>
+        <v>0.002863788193625538</v>
       </c>
       <c r="C21">
-        <v>0.7557691969524982</v>
+        <v>0.9577681173620121</v>
       </c>
       <c r="D21">
-        <v>0.09719750251701564</v>
+        <v>0.002816125596958879</v>
       </c>
       <c r="E21">
-        <v>0.75331847927089</v>
+        <v>0.9573220784948555</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1183,16 +1183,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.1920676360627294</v>
+        <v>0.05843052567054752</v>
       </c>
       <c r="C22">
-        <v>0.6644033275932151</v>
+        <v>0.8109326024898164</v>
       </c>
       <c r="D22">
-        <v>0.1891692862752684</v>
+        <v>0.05748467407373454</v>
       </c>
       <c r="E22">
-        <v>0.6612012847580109</v>
+        <v>0.8089939779468382</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1200,16 +1200,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>0.01194982698598857</v>
+        <v>0.06151771313774645</v>
       </c>
       <c r="C23">
-        <v>0.9138578633394601</v>
+        <v>0.8060979356643249</v>
       </c>
       <c r="D23">
-        <v>0.01175183347269261</v>
+        <v>0.06052344511824794</v>
       </c>
       <c r="E23">
-        <v>0.912952440072729</v>
+        <v>0.8041130166389043</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1217,16 +1217,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>1.111698956812139</v>
+        <v>3.249417763346871</v>
       </c>
       <c r="C24">
-        <v>0.2956692808569352</v>
+        <v>0.07249283197090534</v>
       </c>
       <c r="D24">
-        <v>1.103392644631868</v>
+        <v>3.284191725037537</v>
       </c>
       <c r="E24">
-        <v>0.2917129310314215</v>
+        <v>0.07144883366550028</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1251,16 +1251,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>0.4364667218837859</v>
+        <v>0.6516083827540431</v>
       </c>
       <c r="C26">
-        <v>0.5128945647597944</v>
+        <v>0.4237909029605197</v>
       </c>
       <c r="D26">
-        <v>0.4307590430811847</v>
+        <v>0.6442465467952395</v>
       </c>
       <c r="E26">
-        <v>0.5088327668083621</v>
+        <v>0.4195382270835888</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1268,16 +1268,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>1.725405098519945</v>
+        <v>0.1456808553612943</v>
       </c>
       <c r="C27">
-        <v>0.1920596870170024</v>
+        <v>0.7055781827013691</v>
       </c>
       <c r="D27">
-        <v>1.721399272556762</v>
+        <v>0.1434269624600469</v>
       </c>
       <c r="E27">
-        <v>0.1889987742478963</v>
+        <v>0.7026975384972266</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1285,16 +1285,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>13.95988166538526</v>
+        <v>8.608103718776512</v>
       </c>
       <c r="C28">
-        <v>0.3111271452281945</v>
+        <v>0.758776795198184</v>
       </c>
       <c r="D28">
-        <v>1.173853947649917</v>
+        <v>0.6890590254307571</v>
       </c>
       <c r="E28">
-        <v>0.3032775039448466</v>
+        <v>0.7359887623537218</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1302,16 +1302,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>5.036668036364564</v>
+        <v>1.77501126861753</v>
       </c>
       <c r="C29">
-        <v>0.02479212112465107</v>
+        <v>0.1857461149140944</v>
       </c>
       <c r="D29">
-        <v>5.169707750633152</v>
+        <v>1.771633323414906</v>
       </c>
       <c r="E29">
-        <v>0.02481617773228851</v>
+        <v>0.1827631090689849</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1319,16 +1319,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>6.977652636006542</v>
+        <v>0.9029077464808166</v>
       </c>
       <c r="C30">
-        <v>0.007974511914597781</v>
+        <v>0.3461691524538211</v>
       </c>
       <c r="D30">
-        <v>7.284957623443224</v>
+        <v>0.8945903889739054</v>
       </c>
       <c r="E30">
-        <v>0.008253379370031264</v>
+        <v>0.3420032321635251</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1336,16 +1336,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>1.784801688098083</v>
+        <v>0.0003804259832085322</v>
       </c>
       <c r="C31">
-        <v>0.1845284511121745</v>
+        <v>0.9846014862237022</v>
       </c>
       <c r="D31">
-        <v>1.781552644693824</v>
+        <v>0.0003740867360873441</v>
       </c>
       <c r="E31">
-        <v>0.1815608105157722</v>
+        <v>0.9844386377785442</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1353,16 +1353,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>1.104742313040621</v>
+        <v>2.375261226139145</v>
       </c>
       <c r="C32">
-        <v>0.2971923576589294</v>
+        <v>0.1253520727879129</v>
       </c>
       <c r="D32">
-        <v>1.096423822739993</v>
+        <v>2.382839083054389</v>
       </c>
       <c r="E32">
-        <v>0.2932277153838155</v>
+        <v>0.1232709760403845</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1370,16 +1370,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0.8241475863909109</v>
+        <v>0.2110736254977486</v>
       </c>
       <c r="C33">
-        <v>0.3681879547606182</v>
+        <v>0.6492395255244993</v>
       </c>
       <c r="D33">
-        <v>0.8160161074964674</v>
+        <v>0.2079214545330101</v>
       </c>
       <c r="E33">
-        <v>0.3639702931762541</v>
+        <v>0.6459272057400882</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1387,16 +1387,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>2.008086148255788</v>
+        <v>0.8128417951814315</v>
       </c>
       <c r="C34">
-        <v>0.1590832987547657</v>
+        <v>0.3715049118635382</v>
       </c>
       <c r="D34">
-        <v>2.008223765163383</v>
+        <v>0.8047455218840078</v>
       </c>
       <c r="E34">
-        <v>0.1564625901619222</v>
+        <v>0.3672814047108148</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1404,16 +1404,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>4.477067510117103</v>
+        <v>0.4249548994368624</v>
       </c>
       <c r="C35">
-        <v>0.03454012572649992</v>
+        <v>0.518515800156883</v>
       </c>
       <c r="D35">
-        <v>4.573065752465072</v>
+        <v>0.4193573842383083</v>
       </c>
       <c r="E35">
-        <v>0.03435261590765105</v>
+        <v>0.5144749434314021</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1421,16 +1421,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.6952060835462381</v>
+        <v>0.01208350480399023</v>
       </c>
       <c r="C36">
-        <v>0.4086552062091686</v>
+        <v>0.9133792477318097</v>
       </c>
       <c r="D36">
-        <v>0.6876028629319244</v>
+        <v>0.0118833096574963</v>
       </c>
       <c r="E36">
-        <v>0.4043992234432632</v>
+        <v>0.9124688585172541</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1438,16 +1438,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>5.810508536553787</v>
+        <v>0.4284342773422267</v>
       </c>
       <c r="C37">
-        <v>0.01573748633183372</v>
+        <v>0.5168055567509965</v>
       </c>
       <c r="D37">
-        <v>6.004405471346108</v>
+        <v>0.4228032343713162</v>
       </c>
       <c r="E37">
-        <v>0.01593068684403745</v>
+        <v>0.5127582262213521</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1472,16 +1472,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>2.059777799223328</v>
+        <v>0.03322316164639183</v>
       </c>
       <c r="C39">
-        <v>0.1537741580216738</v>
+        <v>0.856856713597863</v>
       </c>
       <c r="D39">
-        <v>2.060821794066049</v>
+        <v>0.03267848964181263</v>
       </c>
       <c r="E39">
-        <v>0.1512322217299361</v>
+        <v>0.8553690998605935</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1489,16 +1489,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>5.402583316974501</v>
+        <v>0.3035429025127856</v>
       </c>
       <c r="C40">
-        <v>0.01998792294866056</v>
+        <v>0.5853918139688385</v>
       </c>
       <c r="D40">
-        <v>5.562994785181921</v>
+        <v>0.2992407909562096</v>
       </c>
       <c r="E40">
-        <v>0.02010696889523925</v>
+        <v>0.5816698169483802</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1506,16 +1506,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>10.51535389271052</v>
+        <v>8.69945652767699</v>
       </c>
       <c r="C41">
-        <v>0.5929043646814095</v>
+        <v>0.7512979243539746</v>
       </c>
       <c r="D41">
-        <v>0.8563931918951768</v>
+        <v>0.6969431740263017</v>
       </c>
       <c r="E41">
-        <v>0.5708441387023735</v>
+        <v>0.7283638242811632</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1523,16 +1523,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>0.0236791279590598</v>
+        <v>0.4934087373349971</v>
       </c>
       <c r="C42">
-        <v>0.8789683934682</v>
+        <v>0.4865573203709869</v>
       </c>
       <c r="D42">
-        <v>0.02328907136724493</v>
+        <v>0.487188450363895</v>
       </c>
       <c r="E42">
-        <v>0.8777041654924456</v>
+        <v>0.4824106723545271</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1540,16 +1540,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>0.2402577319677679</v>
+        <v>0.161685281039623</v>
       </c>
       <c r="C43">
-        <v>0.6274822689172502</v>
+        <v>0.6906106471600749</v>
       </c>
       <c r="D43">
-        <v>0.2367273996694605</v>
+        <v>0.1592050356133492</v>
       </c>
       <c r="E43">
-        <v>0.6240200291231011</v>
+        <v>0.6876096356892305</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1557,16 +1557,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>0.05335751233392472</v>
+        <v>0.09348565619113902</v>
       </c>
       <c r="C44">
-        <v>0.8191797603765786</v>
+        <v>0.762184882097621</v>
       </c>
       <c r="D44">
-        <v>0.0524915606208004</v>
+        <v>0.09199923366068179</v>
       </c>
       <c r="E44">
-        <v>0.8173206668303463</v>
+        <v>0.7597917709214268</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1574,16 +1574,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>0.1294381045524817</v>
+        <v>0.8998760218275592</v>
       </c>
       <c r="C45">
-        <v>0.7217616100495756</v>
+        <v>0.3469831986934054</v>
       </c>
       <c r="D45">
-        <v>0.12741824260835</v>
+        <v>0.891563896231656</v>
       </c>
       <c r="E45">
-        <v>0.7190153440988892</v>
+        <v>0.3428149564238898</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1591,16 +1591,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>1.430568637181131</v>
+        <v>0.01533722305593788</v>
       </c>
       <c r="C46">
-        <v>0.2351891805482938</v>
+        <v>0.9024625082137404</v>
       </c>
       <c r="D46">
-        <v>1.423698311167822</v>
+        <v>0.01508353050060944</v>
       </c>
       <c r="E46">
-        <v>0.2316716590228891</v>
+        <v>0.9014391551181914</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1608,16 +1608,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>1.890382922084299</v>
+        <v>0.6984787637147827</v>
       </c>
       <c r="C47">
-        <v>0.1719612684158524</v>
+        <v>0.4075511854460979</v>
       </c>
       <c r="D47">
-        <v>1.888628465019864</v>
+        <v>0.6908587020873331</v>
       </c>
       <c r="E47">
-        <v>0.1691587381707257</v>
+        <v>0.4032953242485754</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1625,16 +1625,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>4.046088090970406</v>
+        <v>0.3139055201216445</v>
       </c>
       <c r="C48">
-        <v>0.04469234679838346</v>
+        <v>0.5790508429749114</v>
       </c>
       <c r="D48">
-        <v>4.117484152747485</v>
+        <v>0.309483332506778</v>
       </c>
       <c r="E48">
-        <v>0.04427382859001437</v>
+        <v>0.5752934322878471</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1642,16 +1642,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>0.7583919254390059</v>
+        <v>0.1235956422891649</v>
       </c>
       <c r="C49">
-        <v>0.3880775824939857</v>
+        <v>0.7278615062559204</v>
       </c>
       <c r="D49">
-        <v>0.750495138792865</v>
+        <v>0.1216610213516351</v>
       </c>
       <c r="E49">
-        <v>0.3838322344162485</v>
+        <v>0.7251669784029728</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1659,16 +1659,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>0.07674271562881696</v>
+        <v>2.270700681801356</v>
       </c>
       <c r="C50">
-        <v>0.7839547438418863</v>
+        <v>0.1340698543786043</v>
       </c>
       <c r="D50">
-        <v>0.07551196197687224</v>
+        <v>2.275921813892434</v>
       </c>
       <c r="E50">
-        <v>0.7817610969543161</v>
+        <v>0.1318402833668136</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1693,16 +1693,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>1.784324436595326</v>
+        <v>0.01625904283593993</v>
       </c>
       <c r="C52">
-        <v>0.1845875953652593</v>
+        <v>0.8995889910816609</v>
       </c>
       <c r="D52">
-        <v>1.781069071548977</v>
+        <v>0.01599022533665911</v>
       </c>
       <c r="E52">
-        <v>0.1816192058943721</v>
+        <v>0.898536005632299</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1710,16 +1710,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>0.02344999889929422</v>
+        <v>0.651171231863743</v>
       </c>
       <c r="C53">
-        <v>0.8795509595817111</v>
+        <v>0.4239468388920307</v>
       </c>
       <c r="D53">
-        <v>0.02306367261011185</v>
+        <v>0.6438119766487086</v>
       </c>
       <c r="E53">
-        <v>0.8782926633191156</v>
+        <v>0.4196942446372449</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1727,16 +1727,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>36.49105815966952</v>
+        <v>19.56004560734998</v>
       </c>
       <c r="C54">
-        <v>5.868594327119544E-05</v>
+        <v>0.0688873341417436</v>
       </c>
       <c r="D54">
-        <v>3.896332473543316</v>
+        <v>1.736464415183966</v>
       </c>
       <c r="E54">
-        <v>0.0002700445635616415</v>
+        <v>0.07587967529417443</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1744,16 +1744,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>0.9571946557041366</v>
+        <v>0.08694934619202233</v>
       </c>
       <c r="C55">
-        <v>0.3320150588535583</v>
+        <v>0.7704103118352563</v>
       </c>
       <c r="D55">
-        <v>0.9488097079568714</v>
+        <v>0.08556218689055806</v>
       </c>
       <c r="E55">
-        <v>0.3278946957683463</v>
+        <v>0.768091856729335</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1761,16 +1761,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>0.01902033733284902</v>
+        <v>2.422362503687494</v>
       </c>
       <c r="C56">
-        <v>0.8914449164761618</v>
+        <v>0.1216301711030297</v>
       </c>
       <c r="D56">
-        <v>0.01870629671125004</v>
+        <v>2.431064116627526</v>
       </c>
       <c r="E56">
-        <v>0.8903081968132394</v>
+        <v>0.1196144142436582</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1778,16 +1778,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>0.6163746580704332</v>
+        <v>0.003316972212830116</v>
       </c>
       <c r="C57">
-        <v>0.4366404617668405</v>
+        <v>0.9545525820122297</v>
       </c>
       <c r="D57">
-        <v>0.6092310351942898</v>
+        <v>0.003261779502887134</v>
       </c>
       <c r="E57">
-        <v>0.4323976847375377</v>
+        <v>0.9540726972332276</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1795,16 +1795,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>1.363822683097529</v>
+        <v>0.002267917804474884</v>
       </c>
       <c r="C58">
-        <v>0.2464926069083438</v>
+        <v>0.9624140674738667</v>
       </c>
       <c r="D58">
-        <v>1.356509289536757</v>
+        <v>0.002230161322922428</v>
       </c>
       <c r="E58">
-        <v>0.2428760743815118</v>
+        <v>0.962016971954007</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1812,16 +1812,16 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>0.04458477848102049</v>
+        <v>0.01217583532544531</v>
       </c>
       <c r="C59">
-        <v>0.8344791650890286</v>
+        <v>0.9130502327505459</v>
       </c>
       <c r="D59">
-        <v>0.04385799383082777</v>
+        <v>0.01197411969427259</v>
       </c>
       <c r="E59">
-        <v>0.8327693827598772</v>
+        <v>0.9121364304163414</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1829,16 +1829,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>3.052644975875451</v>
+        <v>0.614897147249196</v>
       </c>
       <c r="C60">
-        <v>0.0818499680944343</v>
+        <v>0.4371920932172557</v>
       </c>
       <c r="D60">
-        <v>3.080121881157524</v>
+        <v>0.6077631265677892</v>
       </c>
       <c r="E60">
-        <v>0.08060577129247931</v>
+        <v>0.4329498832711762</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1846,16 +1846,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>18.98618962694745</v>
+        <v>0.8464671656642597</v>
       </c>
       <c r="C61">
-        <v>6.834629103096174E-06</v>
+        <v>0.361758582225409</v>
       </c>
       <c r="D61">
-        <v>22.17885225501268</v>
+        <v>0.8382724638744348</v>
       </c>
       <c r="E61">
-        <v>1.316680093407071E-05</v>
+        <v>0.3575536844187734</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1863,16 +1863,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>1.326801542154676</v>
+        <v>1.835230427351897</v>
       </c>
       <c r="C62">
-        <v>0.2530452382139192</v>
+        <v>0.1783996159204373</v>
       </c>
       <c r="D62">
-        <v>1.319274983810813</v>
+        <v>1.832671372446455</v>
       </c>
       <c r="E62">
-        <v>0.249375024770454</v>
+        <v>0.1755110006994</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1880,16 +1880,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>0.7035403260245854</v>
+        <v>0.08548608195223295</v>
       </c>
       <c r="C63">
-        <v>0.4058522205486469</v>
+        <v>0.7722972801426462</v>
       </c>
       <c r="D63">
-        <v>0.6958945696945169</v>
+        <v>0.08412124054688533</v>
       </c>
       <c r="E63">
-        <v>0.4015966443276455</v>
+        <v>0.7699960752195893</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1914,16 +1914,16 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>2.913184041880115</v>
+        <v>3.496845888581768</v>
       </c>
       <c r="C65">
-        <v>0.08925609985397694</v>
+        <v>0.06230490794734175</v>
       </c>
       <c r="D65">
-        <v>2.935904560465705</v>
+        <v>3.54177376569591</v>
       </c>
       <c r="E65">
-        <v>0.08785826281426258</v>
+        <v>0.06148582705696494</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1931,16 +1931,16 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>1.933773986027369</v>
+        <v>3.094703461311101</v>
       </c>
       <c r="C66">
-        <v>0.1670812990078569</v>
+        <v>0.07974724638299152</v>
       </c>
       <c r="D66">
-        <v>1.932689288503422</v>
+        <v>3.123682324468999</v>
       </c>
       <c r="E66">
-        <v>0.1643461426039929</v>
+        <v>0.07854746191615967</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1948,16 +1948,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>11.51309654310563</v>
+        <v>16.39459099011964</v>
       </c>
       <c r="C67">
-        <v>0.5044892157249741</v>
+        <v>0.1720554554534182</v>
       </c>
       <c r="D67">
-        <v>0.9462749963806925</v>
+        <v>1.410979449743714</v>
       </c>
       <c r="E67">
-        <v>0.4855314004542135</v>
+        <v>0.173824014804435</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1965,16 +1965,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>0.1745227925831117</v>
+        <v>0.2860753128992721</v>
       </c>
       <c r="C68">
-        <v>0.679213155158841</v>
+        <v>0.596404713058128</v>
       </c>
       <c r="D68">
-        <v>0.1718640309619562</v>
+        <v>0.2819796194164176</v>
       </c>
       <c r="E68">
-        <v>0.6761231460819512</v>
+        <v>0.5927466094595566</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1982,16 +1982,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>0.3638664129151259</v>
+        <v>0.7455469420048244</v>
       </c>
       <c r="C69">
-        <v>0.5502716513184061</v>
+        <v>0.3921386348957607</v>
       </c>
       <c r="D69">
-        <v>0.3588902068013652</v>
+        <v>0.7377044370308418</v>
       </c>
       <c r="E69">
-        <v>0.5463667306446803</v>
+        <v>0.3878897680132886</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1999,16 +1999,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>0.04174527685949503</v>
+        <v>2.421106022332253E-06</v>
       </c>
       <c r="C70">
-        <v>0.8397637942245273</v>
+        <v>0.9987714945963323</v>
       </c>
       <c r="D70">
-        <v>0.04106380741191878</v>
+        <v>2.380754299620651E-06</v>
       </c>
       <c r="E70">
-        <v>0.8381060913443286</v>
+        <v>0.9987584998103453</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2016,16 +2016,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>0.4309169058131745</v>
+        <v>2.281842736363968</v>
       </c>
       <c r="C71">
-        <v>0.5155912519751493</v>
+        <v>0.1331098016318809</v>
       </c>
       <c r="D71">
-        <v>0.4252620624840048</v>
+        <v>2.287305961542805</v>
       </c>
       <c r="E71">
-        <v>0.5115393792088616</v>
+        <v>0.1308962691054729</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2033,16 +2033,16 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>0.1457365492671414</v>
+        <v>0.1274315812949878</v>
       </c>
       <c r="C72">
-        <v>0.7055245041084213</v>
+        <v>0.7238387829470441</v>
       </c>
       <c r="D72">
-        <v>0.1434818613740082</v>
+        <v>0.1254409310751201</v>
       </c>
       <c r="E72">
-        <v>0.7026434213672417</v>
+        <v>0.7211100698757404</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2050,16 +2050,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>0.03407019135780232</v>
+        <v>6.471038864107319</v>
       </c>
       <c r="C73">
-        <v>0.8550631657771266</v>
+        <v>0.01070492275237219</v>
       </c>
       <c r="D73">
-        <v>0.0335118694668813</v>
+        <v>6.725883671662117</v>
       </c>
       <c r="E73">
-        <v>0.8535575923515002</v>
+        <v>0.01096464196826856</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2067,16 +2067,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>1.926178303689734</v>
+        <v>0.1278097177605542</v>
       </c>
       <c r="C74">
-        <v>0.1679240890101471</v>
+        <v>0.7234459340131898</v>
       </c>
       <c r="D74">
-        <v>1.924974025317679</v>
+        <v>0.1258135574250838</v>
       </c>
       <c r="E74">
-        <v>0.165177164823034</v>
+        <v>0.7207138960229136</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2084,16 +2084,16 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>0.6797490950942864</v>
+        <v>3.059137706179329</v>
       </c>
       <c r="C75">
-        <v>0.4139290126628881</v>
+        <v>0.08152154700447153</v>
       </c>
       <c r="D75">
-        <v>0.6722278289965228</v>
+        <v>3.086844429299505</v>
       </c>
       <c r="E75">
-        <v>0.4096731357010943</v>
+        <v>0.08028426425861719</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2101,16 +2101,16 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>0.4032354634762259</v>
+        <v>1.064109842682579</v>
       </c>
       <c r="C76">
-        <v>0.5294205445147973</v>
+        <v>0.3062912285704776</v>
       </c>
       <c r="D76">
-        <v>0.3978517719487644</v>
+        <v>1.055736508722961</v>
       </c>
       <c r="E76">
-        <v>0.5254230415980563</v>
+        <v>0.3022796933282824</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2135,16 +2135,16 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>0.5443236988072986</v>
+        <v>0.1531842148711871</v>
       </c>
       <c r="C78">
-        <v>0.4648456716828674</v>
+        <v>0.6984492503227698</v>
       </c>
       <c r="D78">
-        <v>0.5376906183789304</v>
+        <v>0.1508236763437125</v>
       </c>
       <c r="E78">
-        <v>0.4606463485732204</v>
+        <v>0.6955107929824831</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2152,16 +2152,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>0.001124714561084872</v>
+        <v>0.7838648900294354</v>
       </c>
       <c r="C79">
-        <v>0.9735264119773693</v>
+        <v>0.3801981975750962</v>
       </c>
       <c r="D79">
-        <v>0.001105979684335188</v>
+        <v>0.7758686098836391</v>
       </c>
       <c r="E79">
-        <v>0.9732465486228018</v>
+        <v>0.3759617192413737</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2169,16 +2169,16 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>16.72876237841596</v>
+        <v>9.277788557778205</v>
       </c>
       <c r="C80">
-        <v>0.1573682880684978</v>
+        <v>0.7024653785739741</v>
       </c>
       <c r="D80">
-        <v>1.444398278839191</v>
+        <v>0.7471576560471044</v>
       </c>
       <c r="E80">
-        <v>0.1600883524440081</v>
+        <v>0.6790382850851973</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2186,16 +2186,16 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>5.411509130260002</v>
+        <v>0.6921166091231212</v>
       </c>
       <c r="C81">
-        <v>0.0198834135430088</v>
+        <v>0.4097014271377054</v>
       </c>
       <c r="D81">
-        <v>5.572619662969206</v>
+        <v>0.6845294506563512</v>
       </c>
       <c r="E81">
-        <v>0.02000441475830839</v>
+        <v>0.4054453752564919</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2203,16 +2203,16 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>0.06499458088933263</v>
+        <v>3.134060271292012</v>
       </c>
       <c r="C82">
-        <v>0.800804491365644</v>
+        <v>0.07783158844430543</v>
       </c>
       <c r="D82">
-        <v>0.06394597238847473</v>
+        <v>3.164473009595047</v>
       </c>
       <c r="E82">
-        <v>0.7987691726566737</v>
+        <v>0.07667256122162822</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2220,16 +2220,16 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>6.440643258433982</v>
+        <v>2.442222083007248</v>
       </c>
       <c r="C83">
-        <v>0.01089600776906338</v>
+        <v>0.1200973155694103</v>
       </c>
       <c r="D83">
-        <v>6.692499203080021</v>
+        <v>2.451409093478616</v>
       </c>
       <c r="E83">
-        <v>0.01115382498802052</v>
+        <v>0.1181088100210026</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2237,16 +2237,16 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>2.027649180141107</v>
+        <v>0.6841959601781156</v>
       </c>
       <c r="C84">
-        <v>0.1570501718689876</v>
+        <v>0.4124016179695386</v>
       </c>
       <c r="D84">
-        <v>2.028124400284257</v>
+        <v>0.6766507081834094</v>
       </c>
       <c r="E84">
-        <v>0.1544593629305868</v>
+        <v>0.4081455940699449</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2254,16 +2254,16 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>0.002873855877632003</v>
+        <v>1.094105791883933</v>
       </c>
       <c r="C85">
-        <v>0.9576940177247425</v>
+        <v>0.2995404615196757</v>
       </c>
       <c r="D85">
-        <v>0.002826025959593363</v>
+        <v>1.085770258086097</v>
       </c>
       <c r="E85">
-        <v>0.9572471986306081</v>
+        <v>0.2955632852896874</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2271,16 +2271,16 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>1.184511331216664</v>
+        <v>0.07714004702706667</v>
       </c>
       <c r="C86">
-        <v>0.2803049141252081</v>
+        <v>0.7834099179350713</v>
       </c>
       <c r="D86">
-        <v>1.17638145202772</v>
+        <v>0.07590317269587511</v>
       </c>
       <c r="E86">
-        <v>0.2764394881737324</v>
+        <v>0.7812112070650155</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2288,16 +2288,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>1.893222672498811</v>
+        <v>1.871403284358508</v>
       </c>
       <c r="C87">
-        <v>0.1716369939415158</v>
+        <v>0.1741465506104766</v>
       </c>
       <c r="D87">
-        <v>1.891511058128255</v>
+        <v>1.869366044243075</v>
       </c>
       <c r="E87">
-        <v>0.1688388835319597</v>
+        <v>0.1713144461233943</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2305,16 +2305,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>1.43150058848073</v>
+        <v>1.032371402441128</v>
       </c>
       <c r="C88">
-        <v>0.235035819173603</v>
+        <v>0.3136485341669343</v>
       </c>
       <c r="D88">
-        <v>1.424636984351647</v>
+        <v>1.023974562863166</v>
       </c>
       <c r="E88">
-        <v>0.2315196977186709</v>
+        <v>0.3096023435321562</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2322,16 +2322,16 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>1.444412677024487</v>
+        <v>0.02132981373868414</v>
       </c>
       <c r="C89">
-        <v>0.2329232852743652</v>
+        <v>0.885085878811347</v>
       </c>
       <c r="D89">
-        <v>1.437643722556621</v>
+        <v>0.02097804565808808</v>
       </c>
       <c r="E89">
-        <v>0.2294266060485863</v>
+        <v>0.8838840489793131</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2356,16 +2356,16 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>5.605050218798922</v>
+        <v>0.7875435837183709</v>
       </c>
       <c r="C91">
-        <v>0.01774918960443736</v>
+        <v>0.3790789240314929</v>
       </c>
       <c r="D91">
-        <v>5.781688152171923</v>
+        <v>0.7795338312152665</v>
       </c>
       <c r="E91">
-        <v>0.01790878167948545</v>
+        <v>0.3748439268403291</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2373,16 +2373,16 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>0.9877083174541879</v>
+        <v>0.133981002170569</v>
       </c>
       <c r="C92">
-        <v>0.324394821027409</v>
+        <v>0.7171247919972251</v>
       </c>
       <c r="D92">
-        <v>0.9793070935099655</v>
+        <v>0.1318952476132025</v>
       </c>
       <c r="E92">
-        <v>0.3203031274760009</v>
+        <v>0.7143395899318912</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2390,16 +2390,16 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>17.50119255662504</v>
+        <v>7.070330113035714</v>
       </c>
       <c r="C93">
-        <v>0.1271593213776218</v>
+        <v>0.870752821390682</v>
       </c>
       <c r="D93">
-        <v>1.522479179894691</v>
+        <v>0.5582569833449272</v>
       </c>
       <c r="E93">
-        <v>0.1316966571075712</v>
+        <v>0.8529310313656845</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2407,16 +2407,16 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>0.04584381900886836</v>
+        <v>0.01602280672087009</v>
       </c>
       <c r="C94">
-        <v>0.8321921959017752</v>
+        <v>0.9003173358611133</v>
       </c>
       <c r="D94">
-        <v>0.04509698384176559</v>
+        <v>0.01575786398559765</v>
       </c>
       <c r="E94">
-        <v>0.8304599540281279</v>
+        <v>0.8992718570526691</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2424,16 +2424,16 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>0.870129545873346</v>
+        <v>0.3432923907864183</v>
       </c>
       <c r="C95">
-        <v>0.3551091264436347</v>
+        <v>0.5617835046425759</v>
       </c>
       <c r="D95">
-        <v>0.8618769249194536</v>
+        <v>0.3385393340847482</v>
       </c>
       <c r="E95">
-        <v>0.3509194473676754</v>
+        <v>0.5579349286444538</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2441,16 +2441,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>0.03063780258627524</v>
+        <v>0.6414754679518397</v>
       </c>
       <c r="C96">
-        <v>0.8624820172823013</v>
+        <v>0.4274275374666809</v>
       </c>
       <c r="D96">
-        <v>0.03013486642724824</v>
+        <v>0.6341742704601911</v>
       </c>
       <c r="E96">
-        <v>0.8610508945072087</v>
+        <v>0.4231770133809744</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2458,16 +2458,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>0.4739990879842981</v>
+        <v>0.2910708617055313</v>
       </c>
       <c r="C97">
-        <v>0.4952741692184502</v>
+        <v>0.5932120467695948</v>
       </c>
       <c r="D97">
-        <v>0.4679474922223809</v>
+        <v>0.2869156204845285</v>
       </c>
       <c r="E97">
-        <v>0.4911531311355252</v>
+        <v>0.5895351128180191</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2475,16 +2475,16 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>0.1340973187968331</v>
+        <v>0.04683679687690567</v>
       </c>
       <c r="C98">
-        <v>0.7170072441853967</v>
+        <v>0.8304115492440101</v>
       </c>
       <c r="D98">
-        <v>0.1320098815766644</v>
+        <v>0.04607416664882638</v>
       </c>
       <c r="E98">
-        <v>0.7142210595207883</v>
+        <v>0.8286618536361428</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2492,16 +2492,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>0.1562262218349408</v>
+        <v>1.551333177318437</v>
       </c>
       <c r="C99">
-        <v>0.6956161698817109</v>
+        <v>0.2162717788691794</v>
       </c>
       <c r="D99">
-        <v>0.153822710979093</v>
+        <v>1.545456946321003</v>
       </c>
       <c r="E99">
-        <v>0.6926549797109418</v>
+        <v>0.2129387356813828</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2509,16 +2509,16 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>1.962938988645275</v>
+        <v>0.3925267011468536</v>
       </c>
       <c r="C100">
-        <v>0.1638894330837023</v>
+        <v>0.5349484197197043</v>
       </c>
       <c r="D100">
-        <v>1.962322669469552</v>
+        <v>0.38725131012171</v>
       </c>
       <c r="E100">
-        <v>0.161199347410289</v>
+        <v>0.5309742416649561</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2526,16 +2526,16 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>1.629531214137692</v>
+        <v>1.005508177749737</v>
       </c>
       <c r="C101">
-        <v>0.2049791904967236</v>
+        <v>0.3200553919877049</v>
       </c>
       <c r="D101">
-        <v>1.624431205185985</v>
+        <v>0.9971046823890359</v>
       </c>
       <c r="E101">
-        <v>0.2017679004808493</v>
+        <v>0.3159813507235276</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2543,16 +2543,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>0.3745592521288721</v>
+        <v>1.039615735645256</v>
       </c>
       <c r="C102">
-        <v>0.5444614792270239</v>
+        <v>0.3119493007701374</v>
       </c>
       <c r="D102">
-        <v>0.3694698341330279</v>
+        <v>1.031222768527136</v>
       </c>
       <c r="E102">
-        <v>0.5405295132999697</v>
+        <v>0.307910858466076</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2577,16 +2577,16 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>0.8671612783498794</v>
+        <v>0.1308601198113202</v>
       </c>
       <c r="C104">
-        <v>0.3559340672180753</v>
+        <v>0.7203004712859041</v>
       </c>
       <c r="D104">
-        <v>0.8589154085748314</v>
+        <v>0.1288195957122069</v>
       </c>
       <c r="E104">
-        <v>0.3517423873759246</v>
+        <v>0.7175418989720608</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2594,16 +2594,16 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>0.5851225162074947</v>
+        <v>0.4178603643924506</v>
       </c>
       <c r="C105">
-        <v>0.448539439130379</v>
+        <v>0.5220338764197288</v>
       </c>
       <c r="D105">
-        <v>0.5781897395645342</v>
+        <v>0.4123318344073822</v>
       </c>
       <c r="E105">
-        <v>0.4443114336997757</v>
+        <v>0.5180066161968175</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2611,16 +2611,16 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>16.08055112432915</v>
+        <v>12.04587078801657</v>
       </c>
       <c r="C106">
-        <v>0.1867906414377248</v>
+        <v>0.4587940108272177</v>
       </c>
       <c r="D106">
-        <v>1.379769771137648</v>
+        <v>0.9949504971279806</v>
       </c>
       <c r="E106">
-        <v>0.187574471268923</v>
+        <v>0.442002763098876</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2628,16 +2628,16 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>7.341501040140708</v>
+        <v>1.931130362913285</v>
       </c>
       <c r="C107">
-        <v>0.006457159017770877</v>
+        <v>0.1673740813205559</v>
       </c>
       <c r="D107">
-        <v>7.689585168760937</v>
+        <v>1.930003933502471</v>
       </c>
       <c r="E107">
-        <v>0.00673805523018236</v>
+        <v>0.1646348305567664</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2645,16 +2645,16 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>1.06077875218666</v>
+        <v>22.95985739562332</v>
       </c>
       <c r="C108">
-        <v>0.3070528939464316</v>
+        <v>5.867721239343217E-07</v>
       </c>
       <c r="D108">
-        <v>1.052402155023592</v>
+        <v>27.91899413966195</v>
       </c>
       <c r="E108">
-        <v>0.3030376368451104</v>
+        <v>1.654197844302013E-06</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2662,16 +2662,16 @@
         <v>112</v>
       </c>
       <c r="B109">
-        <v>6.501654950958544</v>
+        <v>2.608644852561515</v>
       </c>
       <c r="C109">
-        <v>0.01051587414736056</v>
+        <v>0.1080499181387452</v>
       </c>
       <c r="D109">
-        <v>6.759528377983052</v>
+        <v>2.622170024493284</v>
       </c>
       <c r="E109">
-        <v>0.01077741294296143</v>
+        <v>0.1062825497959605</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2679,16 +2679,16 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>1.693272452333408</v>
+        <v>1.933825795385746</v>
       </c>
       <c r="C110">
-        <v>0.196281526411281</v>
+        <v>0.1670755668980064</v>
       </c>
       <c r="D110">
-        <v>1.688882395084756</v>
+        <v>1.932741916918995</v>
       </c>
       <c r="E110">
-        <v>0.1931701491041588</v>
+        <v>0.1643404907204681</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2696,16 +2696,16 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>0.05950892155220711</v>
+        <v>0.4364015004432309</v>
       </c>
       <c r="C111">
-        <v>0.8092287679627138</v>
+        <v>0.5129261142931389</v>
       </c>
       <c r="D111">
-        <v>0.05854613967328492</v>
+        <v>0.4306944395997945</v>
       </c>
       <c r="E111">
-        <v>0.8072738001009481</v>
+        <v>0.5088644311634007</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2713,16 +2713,16 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>1.359222279014505</v>
+        <v>3.646596919115361</v>
       </c>
       <c r="C112">
-        <v>0.2472955685198509</v>
+        <v>0.05688077706852965</v>
       </c>
       <c r="D112">
-        <v>1.351881132311062</v>
+        <v>3.698202416619347</v>
       </c>
       <c r="E112">
-        <v>0.243672312892277</v>
+        <v>0.05618389980193106</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2730,16 +2730,16 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>1.509931921671686</v>
+        <v>0.04380016260279174</v>
       </c>
       <c r="C113">
-        <v>0.2225463682025478</v>
+        <v>0.8359214451215541</v>
       </c>
       <c r="D113">
-        <v>1.503686930447857</v>
+        <v>0.04308588629962994</v>
       </c>
       <c r="E113">
-        <v>0.2191494748147368</v>
+        <v>0.8342258514465721</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2747,16 +2747,16 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>0.004391349199432959</v>
+        <v>0.6742116527231401</v>
       </c>
       <c r="C114">
-        <v>0.947716801683585</v>
+        <v>0.4158426354320043</v>
       </c>
       <c r="D114">
-        <v>0.004318318073130927</v>
+        <v>0.6667207158086738</v>
       </c>
       <c r="E114">
-        <v>0.9471650519392932</v>
+        <v>0.4115870755395203</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2764,16 +2764,16 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>0.7901452203720671</v>
+        <v>0.7573073816032805</v>
       </c>
       <c r="C115">
-        <v>0.3782901377097428</v>
+        <v>0.388418156938221</v>
       </c>
       <c r="D115">
-        <v>0.7821260765417678</v>
+        <v>0.7494150716234368</v>
       </c>
       <c r="E115">
-        <v>0.374056217663792</v>
+        <v>0.3841724864531281</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2798,16 +2798,16 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>4.895323960469704</v>
+        <v>0.5997405678537682</v>
       </c>
       <c r="C117">
-        <v>0.02695067173438843</v>
+        <v>0.4429126792600885</v>
       </c>
       <c r="D117">
-        <v>5.018460128735725</v>
+        <v>0.5927071460591101</v>
       </c>
       <c r="E117">
-        <v>0.02692952045853809</v>
+        <v>0.4386770283177734</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2815,16 +2815,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>0.04882257144400715</v>
+        <v>0.005315794656297612</v>
       </c>
       <c r="C118">
-        <v>0.8269088424684298</v>
+        <v>0.9424848027042395</v>
       </c>
       <c r="D118">
-        <v>0.04802840250420697</v>
+        <v>0.005227429644881326</v>
       </c>
       <c r="E118">
-        <v>0.8251249002939084</v>
+        <v>0.9418781370730287</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2832,16 +2832,16 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>21.43700936146512</v>
+        <v>16.03506316242236</v>
       </c>
       <c r="C119">
-        <v>0.0373547676631942</v>
+        <v>0.1890013570565564</v>
       </c>
       <c r="D119">
-        <v>1.939335094928271</v>
+        <v>1.375264753170002</v>
       </c>
       <c r="E119">
-        <v>0.04433586281944372</v>
+        <v>0.1896353789420092</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2849,16 +2849,16 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>9.247294834956023</v>
+        <v>0.2409253322621341</v>
       </c>
       <c r="C120">
-        <v>0.002142920734318571</v>
+        <v>0.627004009210919</v>
       </c>
       <c r="D120">
-        <v>9.852407567821755</v>
+        <v>0.2373865135966166</v>
       </c>
       <c r="E120">
-        <v>0.00235843559212019</v>
+        <v>0.6235385884780236</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2866,16 +2866,16 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>7.904069777026459</v>
+        <v>2.236769369018954</v>
       </c>
       <c r="C121">
-        <v>0.004661410538192882</v>
+        <v>0.1370410005063074</v>
       </c>
       <c r="D121">
-        <v>8.320375519734739</v>
+        <v>2.241266515278496</v>
       </c>
       <c r="E121">
-        <v>0.004932369936405385</v>
+        <v>0.1347622810400202</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2883,16 +2883,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>6.60952034999601</v>
+        <v>2.729316045650809</v>
       </c>
       <c r="C122">
-        <v>0.009876288137287064</v>
+        <v>0.1001368702377969</v>
       </c>
       <c r="D122">
-        <v>6.878208855865815</v>
+        <v>2.746289887011885</v>
       </c>
       <c r="E122">
-        <v>0.01014349798277777</v>
+        <v>0.09852146865539552</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2900,16 +2900,16 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>3.033028755545937</v>
+        <v>0.1397711150439163</v>
       </c>
       <c r="C123">
-        <v>0.08285080506130219</v>
+        <v>0.7113419372234693</v>
       </c>
       <c r="D123">
-        <v>3.059815855250595</v>
+        <v>0.1376018695159768</v>
       </c>
       <c r="E123">
-        <v>0.08158559034709463</v>
+        <v>0.7085086609790864</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2917,16 +2917,16 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>0.002101152140423501</v>
+        <v>0.07984202129348805</v>
       </c>
       <c r="C124">
-        <v>0.9638213722668346</v>
+        <v>0.7797443009129115</v>
       </c>
       <c r="D124">
-        <v>0.002066169115877611</v>
+        <v>0.07856359323929782</v>
       </c>
       <c r="E124">
-        <v>0.9634391110848128</v>
+        <v>0.7775116128109055</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2934,16 +2934,16 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>3.543568340853556</v>
+        <v>2.923994800251233</v>
       </c>
       <c r="C125">
-        <v>0.06055658603262311</v>
+        <v>0.08865713731739061</v>
       </c>
       <c r="D125">
-        <v>3.590536462980142</v>
+        <v>2.947071740626706</v>
       </c>
       <c r="E125">
-        <v>0.05977673206561374</v>
+        <v>0.08727156136438428</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2951,16 +2951,16 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>0.004828093672339939</v>
+        <v>11.03633847867513</v>
       </c>
       <c r="C126">
-        <v>0.9451823438531817</v>
+        <v>0.0007599544514741782</v>
       </c>
       <c r="D126">
-        <v>0.004747816468654323</v>
+        <v>11.9515802084973</v>
       </c>
       <c r="E126">
-        <v>0.9446039818842333</v>
+        <v>0.0008934314671604997</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2968,16 +2968,16 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>1.440823694833635</v>
+        <v>0.0943803119502018</v>
       </c>
       <c r="C127">
-        <v>0.2335081867081024</v>
+        <v>0.7610836890685125</v>
       </c>
       <c r="D127">
-        <v>1.434028147705338</v>
+        <v>0.09288035739357191</v>
       </c>
       <c r="E127">
-        <v>0.2300060952294005</v>
+        <v>0.7586806508529877</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2985,16 +2985,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>10.90012929329617</v>
+        <v>0.3321790049251927</v>
       </c>
       <c r="C128">
-        <v>0.0008224939754367643</v>
+        <v>0.5681944630352873</v>
       </c>
       <c r="D128">
-        <v>11.78933804666659</v>
+        <v>0.3275493967821701</v>
       </c>
       <c r="E128">
-        <v>0.0009615754806281078</v>
+        <v>0.5643788193409878</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3019,16 +3019,16 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>3.322462218203692</v>
+        <v>0.9830640964849779</v>
       </c>
       <c r="C130">
-        <v>0.06931394932169227</v>
+        <v>0.325539688476925</v>
       </c>
       <c r="D130">
-        <v>3.360120115674933</v>
+        <v>0.9746643408738773</v>
       </c>
       <c r="E130">
-        <v>0.06833940758983903</v>
+        <v>0.3214434991005231</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3036,16 +3036,16 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>16.21408871777444</v>
+        <v>1.348661626884731</v>
       </c>
       <c r="C131">
-        <v>3.626467861255061E-05</v>
+        <v>0.2491508636390119</v>
       </c>
       <c r="D131">
-        <v>18.43470317945795</v>
+        <v>1.341258127843066</v>
       </c>
       <c r="E131">
-        <v>5.657182148810586E-05</v>
+        <v>0.2455122293167025</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3053,16 +3053,16 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>14.55000560567743</v>
+        <v>15.47402857016787</v>
       </c>
       <c r="C132">
-        <v>0.272132502162887</v>
+        <v>0.2178885065623176</v>
       </c>
       <c r="D132">
-        <v>1.230322967100528</v>
+        <v>1.320023654056989</v>
       </c>
       <c r="E132">
-        <v>0.2669719509267245</v>
+        <v>0.2165307065323565</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3070,16 +3070,16 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>0.8966165449352337</v>
+        <v>0.1232933384763824</v>
       </c>
       <c r="C133">
-        <v>0.347861273783642</v>
+        <v>0.7281814861960969</v>
       </c>
       <c r="D133">
-        <v>0.8883102161600087</v>
+        <v>0.1213631433944207</v>
       </c>
       <c r="E133">
-        <v>0.3436905627477955</v>
+        <v>0.7254896883061058</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3087,16 +3087,16 @@
         <v>137</v>
       </c>
       <c r="B134">
-        <v>0.1868357149865663</v>
+        <v>0.06662538142306662</v>
       </c>
       <c r="C134">
-        <v>0.668733099270385</v>
+        <v>0.7983734849428292</v>
       </c>
       <c r="D134">
-        <v>0.1840082807259006</v>
+        <v>0.06555135326529368</v>
       </c>
       <c r="E134">
-        <v>0.665563377534744</v>
+        <v>0.7963151233527264</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3104,16 +3104,16 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>0.2493916329504753</v>
+        <v>0.14603554450066</v>
       </c>
       <c r="C135">
-        <v>0.6210086389839644</v>
+        <v>0.7052365280599919</v>
       </c>
       <c r="D135">
-        <v>0.2457458303506506</v>
+        <v>0.1437765895301335</v>
       </c>
       <c r="E135">
-        <v>0.6175037734749016</v>
+        <v>0.7023530934737181</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3121,16 +3121,16 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>1.888981130929919</v>
+        <v>1.137091797789704</v>
       </c>
       <c r="C136">
-        <v>0.1721215972706319</v>
+        <v>0.2901931551773671</v>
       </c>
       <c r="D136">
-        <v>1.887205576448566</v>
+        <v>1.12883686062033</v>
       </c>
       <c r="E136">
-        <v>0.1693168847498978</v>
+        <v>0.286267685003052</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3138,16 +3138,16 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>0.006474884401894698</v>
+        <v>0.04622329898219313</v>
       </c>
       <c r="C137">
-        <v>0.9365351170376518</v>
+        <v>0.8315093414185684</v>
       </c>
       <c r="D137">
-        <v>0.006367313225336791</v>
+        <v>0.04547042560814312</v>
       </c>
       <c r="E137">
-        <v>0.935866106598795</v>
+        <v>0.8297704027914379</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3155,16 +3155,16 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>2.392069077386707</v>
+        <v>1.45329197079564</v>
       </c>
       <c r="C138">
-        <v>0.124009790611906</v>
+        <v>0.2314837245226548</v>
       </c>
       <c r="D138">
-        <v>2.400043508267852</v>
+        <v>1.446589748503506</v>
       </c>
       <c r="E138">
-        <v>0.1219521231603414</v>
+        <v>0.2280004616389002</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3172,16 +3172,16 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>0.9643621861494722</v>
+        <v>1.244496430311894</v>
       </c>
       <c r="C139">
-        <v>0.3302040858301005</v>
+        <v>0.2683918172824006</v>
       </c>
       <c r="D139">
-        <v>0.9559720101940532</v>
+        <v>1.236579142545831</v>
       </c>
       <c r="E139">
-        <v>0.3260902697513921</v>
+        <v>0.2646062384805303</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3189,16 +3189,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>5.460483961233886</v>
+        <v>1.969620317867862</v>
       </c>
       <c r="C140">
-        <v>0.01931981216482976</v>
+        <v>0.1631679562006937</v>
       </c>
       <c r="D140">
-        <v>5.625456870339158</v>
+        <v>1.96911335991908</v>
       </c>
       <c r="E140">
-        <v>0.01945125864265882</v>
+        <v>0.160488168846448</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3206,16 +3206,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>0.6146793990380672</v>
+        <v>2.081430995933946</v>
       </c>
       <c r="C141">
-        <v>0.4372734794324582</v>
+        <v>0.1516095101315514</v>
       </c>
       <c r="D141">
-        <v>0.6075467965523673</v>
+        <v>2.082868369202622</v>
       </c>
       <c r="E141">
-        <v>0.4330313541309539</v>
+        <v>0.1491003398264063</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3240,16 +3240,16 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>0.129172468541161</v>
+        <v>1.17364730025197</v>
       </c>
       <c r="C143">
-        <v>0.722035554329702</v>
+        <v>0.2825325236028662</v>
       </c>
       <c r="D143">
-        <v>0.1271564700248445</v>
+        <v>1.165485418707339</v>
       </c>
       <c r="E143">
-        <v>0.7192915994200544</v>
+        <v>0.2786530839721497</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3257,16 +3257,16 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>0.3844223764146015</v>
+        <v>0.08213090578387039</v>
       </c>
       <c r="C144">
-        <v>0.5392015333235952</v>
+        <v>0.7766910400996495</v>
       </c>
       <c r="D144">
-        <v>0.3792302082900113</v>
+        <v>0.08081737071963979</v>
       </c>
       <c r="E144">
-        <v>0.5352459066018547</v>
+        <v>0.7744301765548739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>